<commit_message>
Made minor edits to education and history sections
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djyeo/Google Drive/cv/yeodj-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CD579A-EB0E-6F4A-B6A5-08A74C9F609E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E026EC66-A4FD-8445-A263-291249627FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="99">
   <si>
     <t>type</t>
   </si>
@@ -84,18 +84,6 @@
     <t>Vanderbilt University</t>
   </si>
   <si>
-    <t>M.Ed. Child Studies</t>
-  </si>
-  <si>
-    <t>PGDE Primary Education</t>
-  </si>
-  <si>
-    <t>National Institute of Education, Singapore</t>
-  </si>
-  <si>
-    <t>B. Soc. Sci. Psychology, Second Class Honours (Upper)</t>
-  </si>
-  <si>
     <t>National University of Singapore and  University of California Irvine</t>
   </si>
   <si>
@@ -291,9 +279,6 @@
     <t>*Association for Psychological Science* Student Caucus’ Student Grant Competition</t>
   </si>
   <si>
-    <t>Commissioned titles include: *My Pals Are Here! Mathematics Series*: Primary 2 (3rd Edition, 2014) Teacher’s Planning Guide, Primary 3 (3rd Edition, 2015) Teacher’s Planning Guide, Primary 4 (3rd Edition, 2016) Textbook, Workbook, Teacher’s Planning Guide, Primary 6 (3rd Edition, 2018) Textbook and Workbook; *Primary Mathematics* (US Common Core Edition, 2014) – Grades 3 and 4 Textbooks, Workbooks and Teacher’s Guides; *Math in Focus Nelson* (Ontario, Canada) – Reteach Books Grades 1 – 3</t>
-  </si>
-  <si>
     <t>2014</t>
   </si>
   <si>
@@ -321,7 +306,22 @@
     <t>*Honors Thesis: The synchronizing influence of task-irrelevant auditory rhythm on visual processing speed: An exploratory analysis of behavioral markers*</t>
   </si>
   <si>
-    <t>Ph.D. Neuroscience</t>
+    <t>Commissioned titles include: *My Pals Are Here! Mathematics Series*: Primary 2 (3rd Edition, 2014) Teacher’s Planning Guide, Primary 3 (3rd Edition, 2015) Teacher’s Planning Guide, Primary 4 (3rd Edition, 2016) Textbook, Workbook, Teacher’s Planning Guide, Primary 6 (3rd Edition, 2018) Textbook and Workbook; *Primary Mathematics* (US Common Core Edition, 2014) – Grades 3 and 4 Textbooks, Workbooks and Teacher’s Guides; *My Math Path* (Ontario, Canada) – Reteach Books Grades 1 – 3</t>
+  </si>
+  <si>
+    <t>Ph.D. in Neuroscience</t>
+  </si>
+  <si>
+    <t>PGDE in Primary Education</t>
+  </si>
+  <si>
+    <t>National Institute of Education, Nanyang Technological University</t>
+  </si>
+  <si>
+    <t>M.Ed. in Child Studies</t>
+  </si>
+  <si>
+    <t>B. Soc. Sci. in Psychology, Second Class Honours (Upper)</t>
   </si>
 </sst>
 </file>
@@ -372,14 +372,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -695,20 +702,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D849796-8D2F-2144-8637-FA01837A8DE5}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="91.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43" customWidth="1"/>
+    <col min="5" max="5" width="74.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.33203125" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -716,10 +723,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -739,141 +746,132 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>2016</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>2014</v>
-      </c>
-      <c r="C3">
-        <v>2016</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
+      <c r="D3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>2009</v>
-      </c>
-      <c r="C4">
-        <v>2010</v>
+      <c r="B4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2016</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
-        <v>2005</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="3">
         <v>2009</v>
       </c>
+      <c r="C5" s="3">
+        <v>2010</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
+      <c r="B6" s="3">
+        <v>2005</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2009</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>1</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2"/>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -881,135 +879,141 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>9</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3">
-        <v>2013</v>
+        <v>68</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5">
+        <v>2013</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
+      <c r="C16" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17">
-        <v>2006</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>37</v>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2006</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="1" t="s">
-        <v>87</v>
+        <v>34</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>13</v>
       </c>
+      <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1017,7 +1021,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1025,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1033,23 +1037,23 @@
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1057,7 +1061,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1065,7 +1069,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1073,7 +1077,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1081,295 +1085,295 @@
         <v>13</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
+    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3">
         <v>2018</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" t="s">
-        <v>42</v>
-      </c>
-      <c r="F30" t="s">
-        <v>70</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31">
-        <v>2017</v>
-      </c>
-      <c r="C31">
-        <v>2021</v>
-      </c>
       <c r="D31" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>47</v>
+        <v>38</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="3">
+        <v>2017</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="3">
         <v>2016</v>
       </c>
-      <c r="C32">
+      <c r="C33" s="3">
         <v>2019</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33">
+    <row r="34" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="3">
         <v>2016</v>
       </c>
-      <c r="C33">
+      <c r="C34" s="3">
         <v>2021</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" t="s">
-        <v>45</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34">
-        <v>2016</v>
-      </c>
-      <c r="C34">
-        <v>2021</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
-      <c r="C35">
+      <c r="B35" s="3">
         <v>2016</v>
       </c>
+      <c r="C35" s="3">
+        <v>2021</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36">
-        <v>2014</v>
-      </c>
-      <c r="C36">
+      <c r="C36" s="3">
         <v>2016</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>47</v>
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
-      <c r="C37">
+      <c r="B37" s="3">
+        <v>2014</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2016</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="3">
         <v>2012</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38">
+      <c r="D38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3">
         <v>2012</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39">
-        <v>2008</v>
-      </c>
       <c r="D39" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
-      <c r="C40">
-        <v>2007</v>
+      <c r="C40" s="3">
+        <v>2008</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3">
         <v>2007</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>14</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3">
         <v>2007</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="C43">
-        <v>2006</v>
+      <c r="C43" s="3">
+        <v>2007</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
-      <c r="B44">
+      <c r="C44" s="3">
         <v>2006</v>
       </c>
-      <c r="C44">
-        <v>2009</v>
-      </c>
       <c r="D44" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>14</v>
       </c>
-      <c r="B45">
-        <v>2005</v>
-      </c>
-      <c r="C45">
+      <c r="B45" s="3">
+        <v>2006</v>
+      </c>
+      <c r="C45" s="3">
         <v>2009</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="E45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>14</v>
       </c>
-      <c r="C46">
+      <c r="B46" s="3">
         <v>2005</v>
       </c>
+      <c r="C46" s="3">
+        <v>2009</v>
+      </c>
       <c r="D46" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C47" s="3">
+        <v>2005</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>30</v>
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1377,18 +1381,26 @@
         <v>15</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:D29">
-    <sortCondition ref="D18:D29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:D30">
+    <sortCondition ref="D19:D30"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="G44" r:id="rId1" xr:uid="{6EE05B81-C390-B84D-91E1-984AA0C3694A}"/>
-    <hyperlink ref="G33" r:id="rId2" xr:uid="{231A91C9-015B-064D-8A06-7582C48CDDEC}"/>
-    <hyperlink ref="G30" r:id="rId3" xr:uid="{76D486E3-9C15-8245-AB67-6FB92C69B5ED}"/>
-    <hyperlink ref="G45" r:id="rId4" xr:uid="{CE6AAA19-EBBB-6B4B-96CD-8E3C2F52BD5A}"/>
+    <hyperlink ref="G45" r:id="rId1" xr:uid="{6EE05B81-C390-B84D-91E1-984AA0C3694A}"/>
+    <hyperlink ref="G34" r:id="rId2" xr:uid="{231A91C9-015B-064D-8A06-7582C48CDDEC}"/>
+    <hyperlink ref="G31" r:id="rId3" xr:uid="{76D486E3-9C15-8245-AB67-6FB92C69B5ED}"/>
+    <hyperlink ref="G46" r:id="rId4" xr:uid="{CE6AAA19-EBBB-6B4B-96CD-8E3C2F52BD5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cleaned up unnecessary periods
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djyeo/Google Drive/cv/yeodj-cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E026EC66-A4FD-8445-A263-291249627FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC564D22-C0DE-7F46-AAA5-E67DE88EC771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" xr2:uid="{658FACE9-883F-4F49-B936-65547CAA7E51}"/>
   </bookViews>
@@ -204,124 +204,124 @@
     <t>Undergraduate Bursary Award</t>
   </si>
   <si>
+    <t>Mee Toh School, Singapore</t>
+  </si>
+  <si>
+    <t>https://www.moe.gov.sg/careers/teach/teaching-scholarships-awards/moe-teaching-award</t>
+  </si>
+  <si>
+    <t>http://cohass.ntu.edu.sg/programmes/Pages/HIPS2016.aspx</t>
+  </si>
+  <si>
+    <t>http://2018.laschool4education.com/</t>
+  </si>
+  <si>
+    <t>Overseas Exchange Program Grant</t>
+  </si>
+  <si>
+    <t>http://www.usp.nus.edu.sg/</t>
+  </si>
+  <si>
+    <t>Fellowship for tuition, room, and board</t>
+  </si>
+  <si>
+    <t>Travel Award</t>
+  </si>
+  <si>
+    <t>mentoring</t>
+  </si>
+  <si>
+    <t>NeuroImage</t>
+  </si>
+  <si>
+    <t>Developmental Science</t>
+  </si>
+  <si>
+    <t>Child Development</t>
+  </si>
+  <si>
+    <t>Brain Imaging and Behavior</t>
+  </si>
+  <si>
+    <t>Journal of Cognitive Neuroscience</t>
+  </si>
+  <si>
+    <t>NeuroImage Clinical</t>
+  </si>
+  <si>
+    <t>Journal of Neuroscience</t>
+  </si>
+  <si>
+    <t>Admission interviewing panel for the University Scholars Program (*ad-hoc*)</t>
+  </si>
+  <si>
+    <t>Connectivity course: Structural and functional brain connectivity via MRI and fMRI</t>
+  </si>
+  <si>
+    <t>Athinoula A Martinos Center for Biomedical Imaging, Boston, MA</t>
+  </si>
+  <si>
+    <t>Public elementary school teacher</t>
+  </si>
+  <si>
+    <t>Freelance math curriculum contributor</t>
+  </si>
+  <si>
+    <t>Journal of Experimental Psychology: Learning, Memory, and Cognition</t>
+  </si>
+  <si>
+    <t>*Association for Psychological Science* Student Research Award</t>
+  </si>
+  <si>
+    <t>*Association for Psychological Science* Student Caucus’ Student Grant Competition</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>Lead tutor</t>
+  </si>
+  <si>
+    <t>Mathematics coach</t>
+  </si>
+  <si>
+    <t>Edufront Learning Centre, Singapore</t>
+  </si>
+  <si>
+    <t>Math Cognition Conference Invited Participant</t>
+  </si>
+  <si>
+    <t>National Institutes of Health, United States</t>
+  </si>
+  <si>
+    <t>Oodles Learning and OnSponge Pte Ltd, Singapore</t>
+  </si>
+  <si>
+    <t>Olivia Lasala (undergraduate honors student in psychology)</t>
+  </si>
+  <si>
+    <t>*Honors Thesis: The synchronizing influence of task-irrelevant auditory rhythm on visual processing speed: An exploratory analysis of behavioral markers*</t>
+  </si>
+  <si>
+    <t>Commissioned titles include: *My Pals Are Here! Mathematics Series*: Primary 2 (3rd Edition, 2014) Teacher’s Planning Guide, Primary 3 (3rd Edition, 2015) Teacher’s Planning Guide, Primary 4 (3rd Edition, 2016) Textbook, Workbook, Teacher’s Planning Guide, Primary 6 (3rd Edition, 2018) Textbook and Workbook; *Primary Mathematics* (US Common Core Edition, 2014) – Grades 3 and 4 Textbooks, Workbooks and Teacher’s Guides; *My Math Path* (Ontario, Canada) – Reteach Books Grades 1 – 3</t>
+  </si>
+  <si>
+    <t>Ph.D. in Neuroscience</t>
+  </si>
+  <si>
+    <t>PGDE in Primary Education</t>
+  </si>
+  <si>
+    <t>National Institute of Education, Nanyang Technological University</t>
+  </si>
+  <si>
+    <t>M.Ed. in Child Studies</t>
+  </si>
+  <si>
+    <t>B. Soc. Sci. in Psychology, Second Class Honours (Upper)</t>
+  </si>
+  <si>
     <t>Advisor: Gavin R. Price, Ph.D.</t>
-  </si>
-  <si>
-    <t>Mee Toh School, Singapore</t>
-  </si>
-  <si>
-    <t>https://www.moe.gov.sg/careers/teach/teaching-scholarships-awards/moe-teaching-award</t>
-  </si>
-  <si>
-    <t>http://cohass.ntu.edu.sg/programmes/Pages/HIPS2016.aspx</t>
-  </si>
-  <si>
-    <t>http://2018.laschool4education.com/</t>
-  </si>
-  <si>
-    <t>Overseas Exchange Program Grant</t>
-  </si>
-  <si>
-    <t>http://www.usp.nus.edu.sg/</t>
-  </si>
-  <si>
-    <t>Fellowship for tuition, room, and board</t>
-  </si>
-  <si>
-    <t>Travel Award</t>
-  </si>
-  <si>
-    <t>mentoring</t>
-  </si>
-  <si>
-    <t>NeuroImage</t>
-  </si>
-  <si>
-    <t>Developmental Science</t>
-  </si>
-  <si>
-    <t>Child Development</t>
-  </si>
-  <si>
-    <t>Brain Imaging and Behavior</t>
-  </si>
-  <si>
-    <t>Journal of Cognitive Neuroscience</t>
-  </si>
-  <si>
-    <t>NeuroImage Clinical</t>
-  </si>
-  <si>
-    <t>Journal of Neuroscience</t>
-  </si>
-  <si>
-    <t>Admission interviewing panel for the University Scholars Program (*ad-hoc*)</t>
-  </si>
-  <si>
-    <t>Connectivity course: Structural and functional brain connectivity via MRI and fMRI</t>
-  </si>
-  <si>
-    <t>Athinoula A Martinos Center for Biomedical Imaging, Boston, MA</t>
-  </si>
-  <si>
-    <t>Public elementary school teacher</t>
-  </si>
-  <si>
-    <t>Freelance math curriculum contributor</t>
-  </si>
-  <si>
-    <t>Journal of Experimental Psychology: Learning, Memory, and Cognition</t>
-  </si>
-  <si>
-    <t>*Association for Psychological Science* Student Research Award</t>
-  </si>
-  <si>
-    <t>*Association for Psychological Science* Student Caucus’ Student Grant Competition</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>Lead tutor</t>
-  </si>
-  <si>
-    <t>Mathematics coach</t>
-  </si>
-  <si>
-    <t>Edufront Learning Centre, Singapore</t>
-  </si>
-  <si>
-    <t>Math Cognition Conference Invited Participant</t>
-  </si>
-  <si>
-    <t>National Institutes of Health, United States</t>
-  </si>
-  <si>
-    <t>Oodles Learning and OnSponge Pte Ltd, Singapore</t>
-  </si>
-  <si>
-    <t>Olivia Lasala (undergraduate honors student in psychology)</t>
-  </si>
-  <si>
-    <t>*Honors Thesis: The synchronizing influence of task-irrelevant auditory rhythm on visual processing speed: An exploratory analysis of behavioral markers*</t>
-  </si>
-  <si>
-    <t>Commissioned titles include: *My Pals Are Here! Mathematics Series*: Primary 2 (3rd Edition, 2014) Teacher’s Planning Guide, Primary 3 (3rd Edition, 2015) Teacher’s Planning Guide, Primary 4 (3rd Edition, 2016) Textbook, Workbook, Teacher’s Planning Guide, Primary 6 (3rd Edition, 2018) Textbook and Workbook; *Primary Mathematics* (US Common Core Edition, 2014) – Grades 3 and 4 Textbooks, Workbooks and Teacher’s Guides; *My Math Path* (Ontario, Canada) – Reteach Books Grades 1 – 3</t>
-  </si>
-  <si>
-    <t>Ph.D. in Neuroscience</t>
-  </si>
-  <si>
-    <t>PGDE in Primary Education</t>
-  </si>
-  <si>
-    <t>National Institute of Education, Nanyang Technological University</t>
-  </si>
-  <si>
-    <t>M.Ed. in Child Studies</t>
-  </si>
-  <si>
-    <t>B. Soc. Sci. in Psychology, Second Class Honours (Upper)</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
         <v>2016</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>2016</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -792,10 +792,10 @@
         <v>2010</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -809,7 +809,7 @@
         <v>2009</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -820,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -848,13 +848,13 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -865,13 +865,13 @@
         <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="E10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -882,10 +882,10 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -900,7 +900,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
         <v>24</v>
@@ -915,15 +915,15 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" t="s">
         <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>35</v>
@@ -932,7 +932,7 @@
         <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
@@ -947,7 +947,7 @@
         <v>2013</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1021,7 +1021,7 @@
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1029,7 +1029,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1037,7 +1037,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
         <v>13</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>13</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1061,7 +1061,7 @@
         <v>13</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1069,7 +1069,7 @@
         <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>13</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1110,10 +1110,10 @@
         <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1167,7 +1167,7 @@
         <v>41</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1198,13 +1198,13 @@
         <v>2016</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" t="s">
         <v>88</v>
       </c>
-      <c r="E36" t="s">
-        <v>89</v>
-      </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1235,7 +1235,7 @@
         <v>47</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>48</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1288,7 +1288,7 @@
         <v>2007</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
         <v>53</v>
@@ -1339,7 +1339,7 @@
         <v>49</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1359,7 +1359,7 @@
         <v>28</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="17" x14ac:dyDescent="0.2">

</xml_diff>